<commit_message>
Cường ghi thông tin rồi
Cường ghi thông tin rồi
</commit_message>
<xml_diff>
--- a/Lop NM03.xlsx
+++ b/Lop NM03.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>LỚP NHẬP MÔN 03</t>
   </si>
@@ -55,13 +55,16 @@
   </si>
   <si>
     <t>Nguyễn Duy Cường</t>
+  </si>
+  <si>
+    <t>nhoxsazd@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +75,14 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,14 +105,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -404,7 +418,7 @@
   <dimension ref="C4:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,25 +455,33 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>4</v>
       </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>939025482</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>6</v>
       </c>
@@ -475,8 +497,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F23" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Revert "Cường ghi thông tin rồi"
This reverts commit de0e963e360977acdbda3d963057d7f25bdd32bc.
</commit_message>
<xml_diff>
--- a/Lop NM03.xlsx
+++ b/Lop NM03.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>LỚP NHẬP MÔN 03</t>
   </si>
@@ -55,16 +55,13 @@
   </si>
   <si>
     <t>Nguyễn Duy Cường</t>
-  </si>
-  <si>
-    <t>nhoxsazd@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,14 +72,6 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,17 +94,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,7 +404,7 @@
   <dimension ref="C4:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,33 +441,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+      <c r="D22" t="s">
         <v>12</v>
       </c>
-      <c r="E23">
-        <v>939025482</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>6</v>
       </c>
@@ -497,11 +475,8 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F23" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
tâm đã thêm thông tin
tâm đã thêm thông tin
</commit_message>
<xml_diff>
--- a/Lop NM03.xlsx
+++ b/Lop NM03.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>LỚP NHẬP MÔN 03</t>
   </si>
@@ -54,14 +54,17 @@
     <t>EMAIL</t>
   </si>
   <si>
-    <t>Nguyễn Duy Cường</t>
+    <t>Đỗ Hoàng Băng Tâm</t>
+  </si>
+  <si>
+    <t>bangtam.12a3.tts@gmai.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +75,14 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,14 +105,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -404,14 +418,14 @@
   <dimension ref="C4:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
     <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -441,25 +455,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>969382833</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>6</v>
       </c>
@@ -475,8 +495,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F22" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Revert "tâm đã thêm thông tin"
This reverts commit e161594af0a0d0023a14222d68190ac1f5a6fde4.
</commit_message>
<xml_diff>
--- a/Lop NM03.xlsx
+++ b/Lop NM03.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>LỚP NHẬP MÔN 03</t>
   </si>
@@ -54,17 +54,14 @@
     <t>EMAIL</t>
   </si>
   <si>
-    <t>Đỗ Hoàng Băng Tâm</t>
-  </si>
-  <si>
-    <t>bangtam.12a3.tts@gmai.com</t>
+    <t>Nguyễn Duy Cường</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,14 +72,6 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,17 +94,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,14 +404,14 @@
   <dimension ref="C4:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
     <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -455,31 +441,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
-      <c r="E22">
-        <v>969382833</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>6</v>
       </c>
@@ -495,11 +475,8 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F22" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
tâm đã thay đổi thông tin
tâm đã thay đổi thông tin
</commit_message>
<xml_diff>
--- a/Lop NM03.xlsx
+++ b/Lop NM03.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>LỚP NHẬP MÔN 03</t>
   </si>
@@ -54,14 +54,17 @@
     <t>EMAIL</t>
   </si>
   <si>
-    <t>Nguyễn Duy Cường</t>
+    <t>Đỗ Hoàng Băng Tâm</t>
+  </si>
+  <si>
+    <t>bangtam.12a3.tts@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +75,14 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,14 +105,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,15 +417,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" customWidth="1"/>
     <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -441,25 +455,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>969382833</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>6</v>
       </c>
@@ -475,8 +495,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F22" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>